<commit_message>
Created API end points for primary-screening
</commit_message>
<xml_diff>
--- a/database/PRJ-005/primary/screening_results.xlsx
+++ b/database/PRJ-005/primary/screening_results.xlsx
@@ -1,37 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEP-CER-Web-App-Laptop\CEP-CER-Backend\database\PRJ-005\primary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F9ED2D-FDFA-4F06-91FF-F184DEBFF62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+  <si>
+    <t>PMID</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>ExcludedCriteria</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>OBJECTIVE: Investigate the effect of aluminum oxide air abrasion, used for cleaning the surface of human dentin, on the bond strength to resin cements for indirect restorations.
+DATA AND SOURCE: This study followed PRISMA-ScR guidelines for scoping reviews and registered on the Open Science Framework platform.
+STUDY SELECTION: A comprehensive search of four electronic databases: PubMed, Scopus, Embase, and Web of Science, as well as manual searches, was performed to identify relevant studies published through July 2024. Studies focused on in vitro evaluations of oxide particles as a surface cleaning method for sound human dentin and their effect on the bond strength of resin cements for indirect restorations were included. Studies involving glass ionomer cements and temporary cements were excluded.
+RESULTS: A total of seven (7) studies were included in the descriptive analysis and meta-analysis. The overall meta-analysis of air abrasion with aluminum oxide particles (50 µm) showed a statistically significant difference (SMD: 0.94, 95 % CI, 0.43-1.46), favoring the air abrasion group. Additionally, when comparing pumice with air abrasion using aluminum oxide particles, a significant difference was found (SMD: 0.94, 95 % CI, 0.43-1.46), favoring the air abrasion group. The meta-analysis evaluating substrates with immediate dentin sealing (IDS) and air abrasion with alumina particles showed a significant difference in favor of the control group (IDS only - no cleaning method) (SMD: SMD: 0.62, 95 % CI, 1.10-0.15).
+CONCLUSION: Dentin cleaning with 50 µm aluminum oxide particles significantly improves the bond strength to resin cement. In addition, air abrasion provides higher resin cement bond strength than pumice and water cleaning. However, on substrates treated previously with immediate dentin sealing, air abrasion reduced the resin cement bond strength compared to the no cleaning method.
+CLINICAL SIGNIFICANCE: Air abrasion with 50 µm aluminum oxide particles may improve the bond strength of resin cements to sound dentin, supporting its use before cementing indirect restorations. However, when used after immediate dentin sealing, this technique may impair bond strength and should be avoided in such cases.</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>HTTPConnectionPool(host='localhost', port=7860): Max retries exceeded with url: /api/v1/run/primaryscreen-1-1-1 (Caused by NewConnectionError("HTTPConnection(host='localhost', port=7860): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+  </si>
+  <si>
+    <t>AIM: The study evaluated enamel surface roughness after bracket debonding and adhesive removal using three methods: Tungsten carbide burs (TCB), aluminum oxide air abrasion (AO), and sodium bicarbonate air abrasion (SB).
+MATERIALS AND METHODS: A total of 90 extracted premolars were divided equally into three groups based on adhesive removal methods: TCB, AO, and SB. Procedures were performed under a 4× magnifying loupe. Surface roughness (Ra) was measured using a profilometer and atomic force microscopy (AFM) before bonding (T0). Brackets were bonded, debonded after 24 hours, and the adhesive remnant index (ARI) was assessed. After adhesive removal, Ra was re-evaluated (T1), and removal time was recorded. Data were analyzed using IBM Statistical Package for Social Sciences software.
+RESULTS: The results showed no significant difference in ARI among the three groups. All methods led to a significant increase in Ra after adhesive removal (
+CONCLUSION: Sodium bicarbonate air abrasion effectively removes adhesive remnants and produces the lowest surface roughness compared with other methods. Air abrasion offers a promising alternative to rotary handpieces, restoring the enamel surface to a nearly original condition and reducing the risk of permanent tooth damage.
+CLINICAL SIGNIFICANCE: Sodium bicarbonate air abrasion is a fast, minimally invasive method for adhesive remnant removal. It preserves enamel integrity. How to cite this article: Alkahlout AE, El-Gazzar RI, Shamaa MS. Effect of Air Abrasion Techniques vs Tungsten Carbide Burs on Enamel Surface after Orthodontic Adhesive Remnant Removal. J Contemp Dent Pract 2025;26(4):366-372.</t>
+  </si>
+  <si>
+    <t>OBJECTIVE: The purpose of this in vitro study was to investigate the shear bond strength of high translucent monolithic zirconia and titanium alloy (Ti6Al4V) after various surface treatments using resin cement.
+MATERIALS AND METHODS: Ninety Ti6Al4V specimens were randomly allocated into six groups (n = 15 per group): untreated titanium (CT; control), 50-µm alumina airborne-particle abrasion (AB), 9.5% hydrofluoric acid (HF), anodization (AN), AB followed by AN (AB-AN), and HF followed by AN (HF-AN). Representative specimen from each group was examined using a scanning electron microscope and laser confocal microscopy. The specimens were bonded with 50-µm alumina air-abraded high translucent monolithic zirconia specimen using 10-methacryloyloxydecal dihydrogen phosphate (10-MDP)-containing primer and 10-methoxyl methyl methacrylate (MMA)-based resin cement. The failure mode of was classified using a stereomicroscope. Results were analyzed by one-way ANOVA with Tukey's adjustment for multiple comparisons (p &lt; 0.05).
+RESULTS: The mean bond strength of AB (36.9 ± 1.6 MPa) and HF (32.5 ± 3.4 MPa) groups were statistically significantly higher than other groups (p &lt; 0.05). The AN group showed the lowest bond strength (29.55 ± 3.62 MPa); however, there was no significant difference between CT, AN, AB-AN, and HF-AN. The stereomicroscopic analysis revealed that the AN, AB-AN, and HF-AN groups predominantly showed mixed failure modes.
+CONCLUSION: The surface treatment of Ti6Al4V with either 50-µm alumina airborne-particle abrasion or 9.5% hydrofluoric acid improved the bond strength between Ti6Al4V and high translucent monolithic zirconia. Anodization did not improve the bond strength, regardless of the surface treatments.</t>
+  </si>
+  <si>
+    <t>This study evaluated the repair bond strengths of ceramic and hybrid ceramic CAD/CAM restorations following bioactive-glass, silica-coated alumina, and aluminum oxide surface treatments. Shear bond strength (SBS) tests, surface roughness, and scanning electron microscopic (SEM) evaluations were performed on 180 specimens (7×12×2 mm</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +105,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,181 +429,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PMID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Abstract</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Decision</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ExcludedCriteria</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Rationale</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>40617523</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>OBJECTIVE: Investigate the effect of aluminum oxide air abrasion, used for cleaning the surface of human dentin, on the bond strength to resin cements for indirect restorations.
-DATA AND SOURCE: This study followed PRISMA-ScR guidelines for scoping reviews and registered on the Open Science Framework platform.
-STUDY SELECTION: A comprehensive search of four electronic databases: PubMed, Scopus, Embase, and Web of Science, as well as manual searches, was performed to identify relevant studies published through July 2024. Studies focused on in vitro evaluations of oxide particles as a surface cleaning method for sound human dentin and their effect on the bond strength of resin cements for indirect restorations were included. Studies involving glass ionomer cements and temporary cements were excluded.
-RESULTS: A total of seven (7) studies were included in the descriptive analysis and meta-analysis. The overall meta-analysis of air abrasion with aluminum oxide particles (50 µm) showed a statistically significant difference (SMD: 0.94, 95 % CI, 0.43-1.46), favoring the air abrasion group. Additionally, when comparing pumice with air abrasion using aluminum oxide particles, a significant difference was found (SMD: 0.94, 95 % CI, 0.43-1.46), favoring the air abrasion group. The meta-analysis evaluating substrates with immediate dentin sealing (IDS) and air abrasion with alumina particles showed a significant difference in favor of the control group (IDS only - no cleaning method) (SMD: SMD: 0.62, 95 % CI, 1.10-0.15).
-CONCLUSION: Dentin cleaning with 50 µm aluminum oxide particles significantly improves the bond strength to resin cement. In addition, air abrasion provides higher resin cement bond strength than pumice and water cleaning. However, on substrates treated previously with immediate dentin sealing, air abrasion reduced the resin cement bond strength compared to the no cleaning method.
-CLINICAL SIGNIFICANCE: Air abrasion with 50 µm aluminum oxide particles may improve the bond strength of resin cements to sound dentin, supporting its use before cementing indirect restorations. However, when used after immediate dentin sealing, this technique may impair bond strength and should be avoided in such cases.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>INCLUDE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>DUE</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>The abstract describes a prospective, multicenter clinical trial evaluating the safety and effectiveness of the PERIMOUNT Magna Ease Aortic Heart Valve (Model 3300TFX), which is the specific device under evaluation. The study involves the device's intended use for aortic valve replacement in human subjects. It provides relevant clinical safety and performance data, including mortality rates, valve-related adverse events, and hemodynamic performance.</t>
-        </is>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>40583425</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AIM: The study evaluated enamel surface roughness after bracket debonding and adhesive removal using three methods: Tungsten carbide burs (TCB), aluminum oxide air abrasion (AO), and sodium bicarbonate air abrasion (SB).
-MATERIALS AND METHODS: A total of 90 extracted premolars were divided equally into three groups based on adhesive removal methods: TCB, AO, and SB. Procedures were performed under a 4× magnifying loupe. Surface roughness (Ra) was measured using a profilometer and atomic force microscopy (AFM) before bonding (T0). Brackets were bonded, debonded after 24 hours, and the adhesive remnant index (ARI) was assessed. After adhesive removal, Ra was re-evaluated (T1), and removal time was recorded. Data were analyzed using IBM Statistical Package for Social Sciences software.
-RESULTS: The results showed no significant difference in ARI among the three groups. All methods led to a significant increase in Ra after adhesive removal (
-CONCLUSION: Sodium bicarbonate air abrasion effectively removes adhesive remnants and produces the lowest surface roughness compared with other methods. Air abrasion offers a promising alternative to rotary handpieces, restoring the enamel surface to a nearly original condition and reducing the risk of permanent tooth damage.
-CLINICAL SIGNIFICANCE: Sodium bicarbonate air abrasion is a fast, minimally invasive method for adhesive remnant removal. It preserves enamel integrity. How to cite this article: Alkahlout AE, El-Gazzar RI, Shamaa MS. Effect of Air Abrasion Techniques vs Tungsten Carbide Burs on Enamel Surface after Orthodontic Adhesive Remnant Removal. J Contemp Dent Pract 2025;26(4):366-372.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>EXCLUDE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Literature contains insufficient information to undertake a scientific analysis about device performance.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>The abstract content is missing. Without the abstract, it is impossible to assess the study type, scientific validity, or relevance to the device. Therefore, there is insufficient information to perform a scientific analysis.</t>
-        </is>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>40426153</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>OBJECTIVE: The purpose of this in vitro study was to investigate the shear bond strength of high translucent monolithic zirconia and titanium alloy (Ti6Al4V) after various surface treatments using resin cement.
-MATERIALS AND METHODS: Ninety Ti6Al4V specimens were randomly allocated into six groups (n = 15 per group): untreated titanium (CT; control), 50-µm alumina airborne-particle abrasion (AB), 9.5% hydrofluoric acid (HF), anodization (AN), AB followed by AN (AB-AN), and HF followed by AN (HF-AN). Representative specimen from each group was examined using a scanning electron microscope and laser confocal microscopy. The specimens were bonded with 50-µm alumina air-abraded high translucent monolithic zirconia specimen using 10-methacryloyloxydecal dihydrogen phosphate (10-MDP)-containing primer and 10-methoxyl methyl methacrylate (MMA)-based resin cement. The failure mode of was classified using a stereomicroscope. Results were analyzed by one-way ANOVA with Tukey's adjustment for multiple comparisons (p &lt; 0.05).
-RESULTS: The mean bond strength of AB (36.9 ± 1.6 MPa) and HF (32.5 ± 3.4 MPa) groups were statistically significantly higher than other groups (p &lt; 0.05). The AN group showed the lowest bond strength (29.55 ± 3.62 MPa); however, there was no significant difference between CT, AN, AB-AN, and HF-AN. The stereomicroscopic analysis revealed that the AN, AB-AN, and HF-AN groups predominantly showed mixed failure modes.
-CONCLUSION: The surface treatment of Ti6Al4V with either 50-µm alumina airborne-particle abrasion or 9.5% hydrofluoric acid improved the bond strength between Ti6Al4V and high translucent monolithic zirconia. Anodization did not improve the bond strength, regardless of the surface treatments.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>INCLUDE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>DUE</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>The abstract and IFU are empty. Based on the abstract completeness rule, the article is included as a proper evaluation cannot be made from the provided text. Insufficient information is available to determine the study type, device relevance, or publication validity.</t>
-        </is>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>40358426</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>This study evaluated the repair bond strengths of ceramic and hybrid ceramic CAD/CAM restorations following bioactive-glass, silica-coated alumina, and aluminum oxide surface treatments. Shear bond strength (SBS) tests, surface roughness, and scanning electron microscopic (SEM) evaluations were performed on 180 specimens (7×12×2 mm</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>EXCLUDE</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Literature contains insufficient information to undertake a scientific analysis about device performance.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>The abstract and IFU summary were not provided in the prompt. Without the necessary content, it is impossible to perform the requested analysis of the abstract against the IFU. The submission lacks the required information to make a scientific or relevance-based assessment.</t>
-        </is>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>